<commit_message>
feat: Add perfume filter test with dynamic content validation
</commit_message>
<xml_diff>
--- a/output/registeration_validation_results.xlsx
+++ b/output/registeration_validation_results.xlsx
@@ -32,7 +32,7 @@
     <t>הצליח ✓</t>
   </si>
   <si>
-    <t>01/12/2025 19:31:05</t>
+    <t>01/12/2025 22:34:39</t>
   </si>
   <si>
     <t>נפתח בהצלחה</t>
@@ -41,7 +41,7 @@
     <t>מציאת אזור התחבר/הרשם</t>
   </si>
   <si>
-    <t>01/12/2025 19:31:09</t>
+    <t>01/12/2025 22:34:43</t>
   </si>
   <si>
     <t>נמצא בהצלחה</t>
@@ -50,19 +50,19 @@
     <t>פתיחת תפריט</t>
   </si>
   <si>
-    <t>01/12/2025 19:31:11</t>
+    <t>01/12/2025 22:34:45</t>
   </si>
   <si>
     <t>מציאת כפתור הרשמה</t>
   </si>
   <si>
-    <t>01/12/2025 19:31:16</t>
+    <t>01/12/2025 22:34:50</t>
   </si>
   <si>
     <t>לחיצה על כפתור הרשמה</t>
   </si>
   <si>
-    <t>01/12/2025 19:31:21</t>
+    <t>01/12/2025 22:34:55</t>
   </si>
   <si>
     <t>בוצעה בהצלחה</t>
@@ -77,7 +77,7 @@
     <t>מילוי שדות</t>
   </si>
   <si>
-    <t>01/12/2025 19:31:40</t>
+    <t>01/12/2025 22:35:16</t>
   </si>
   <si>
     <t>כל 12 השדות + 2 צ'קבוקסים מולאו</t>
@@ -86,73 +86,73 @@
     <t>לחיצה על כפתור</t>
   </si>
   <si>
-    <t>01/12/2025 19:31:48</t>
+    <t>01/12/2025 22:35:25</t>
   </si>
   <si>
     <t>טסט 1: הרשמה מוצלחת</t>
   </si>
   <si>
-    <t>01/12/2025 19:31:53</t>
+    <t>01/12/2025 22:35:30</t>
   </si>
   <si>
     <t>ההרשמה הושלמה בהצלחה</t>
   </si>
   <si>
-    <t>01/12/2025 19:32:02</t>
-  </si>
-  <si>
-    <t>01/12/2025 19:32:06</t>
-  </si>
-  <si>
-    <t>01/12/2025 19:32:08</t>
-  </si>
-  <si>
-    <t>01/12/2025 19:32:13</t>
-  </si>
-  <si>
-    <t>01/12/2025 19:32:18</t>
+    <t>01/12/2025 22:35:40</t>
+  </si>
+  <si>
+    <t>01/12/2025 22:35:44</t>
+  </si>
+  <si>
+    <t>01/12/2025 22:35:46</t>
+  </si>
+  <si>
+    <t>01/12/2025 22:35:50</t>
+  </si>
+  <si>
+    <t>01/12/2025 22:35:57</t>
   </si>
   <si>
     <t>מילוי טופס עם אימייל קיים</t>
   </si>
   <si>
-    <t>01/12/2025 19:32:37</t>
+    <t>01/12/2025 22:36:18</t>
   </si>
   <si>
     <t>הטופס מולא עם פרטים שונים ואימייל קיים</t>
   </si>
   <si>
-    <t>01/12/2025 19:32:40</t>
+    <t>01/12/2025 22:36:21</t>
   </si>
   <si>
     <t>בדיקת אימייל כפול</t>
   </si>
   <si>
-    <t>01/12/2025 19:32:45</t>
+    <t>01/12/2025 22:36:26</t>
   </si>
   <si>
     <t>✓ המערכת זיהתה אימייל קיים והציגה שגיאה: "יש לבחור יישוב ורחוב." - הבדיקה עברה בהצלחה!</t>
   </si>
   <si>
-    <t>01/12/2025 19:33:00</t>
-  </si>
-  <si>
-    <t>01/12/2025 19:33:04</t>
-  </si>
-  <si>
-    <t>01/12/2025 19:33:06</t>
-  </si>
-  <si>
-    <t>01/12/2025 19:33:11</t>
-  </si>
-  <si>
-    <t>01/12/2025 19:33:16</t>
+    <t>01/12/2025 22:36:36</t>
+  </si>
+  <si>
+    <t>01/12/2025 22:36:40</t>
+  </si>
+  <si>
+    <t>01/12/2025 22:36:42</t>
+  </si>
+  <si>
+    <t>01/12/2025 22:36:47</t>
+  </si>
+  <si>
+    <t>01/12/2025 22:36:52</t>
   </si>
   <si>
     <t>מילוי טופס עם שדות חסרים</t>
   </si>
   <si>
-    <t>01/12/2025 19:33:34</t>
+    <t>01/12/2025 22:37:13</t>
   </si>
   <si>
     <t>הטופס מולא בלי אימייל וסיסמה</t>
@@ -161,7 +161,7 @@
     <t>ניסיון שליחה עם שדות חסרים</t>
   </si>
   <si>
-    <t>01/12/2025 19:33:38</t>
+    <t>01/12/2025 22:37:16</t>
   </si>
   <si>
     <t>לחיצה בוצעה</t>
@@ -170,31 +170,31 @@
     <t>אימות שדות חובה</t>
   </si>
   <si>
-    <t>01/12/2025 19:33:42</t>
+    <t>01/12/2025 22:37:20</t>
   </si>
   <si>
     <t>✓ המערכת מנעה שליחת טופס עם שדות חובה חסרים: "אנא הזן כתובת אימייל." - הבדיקה עברה!</t>
   </si>
   <si>
-    <t>01/12/2025 19:34:00</t>
-  </si>
-  <si>
-    <t>01/12/2025 19:34:04</t>
-  </si>
-  <si>
-    <t>01/12/2025 19:34:06</t>
-  </si>
-  <si>
-    <t>01/12/2025 19:34:11</t>
-  </si>
-  <si>
-    <t>01/12/2025 19:34:16</t>
+    <t>01/12/2025 22:37:30</t>
+  </si>
+  <si>
+    <t>01/12/2025 22:37:34</t>
+  </si>
+  <si>
+    <t>01/12/2025 22:37:37</t>
+  </si>
+  <si>
+    <t>01/12/2025 22:37:41</t>
+  </si>
+  <si>
+    <t>01/12/2025 22:37:52</t>
   </si>
   <si>
     <t>מילוי טופס עם טלפון שני לא תקין</t>
   </si>
   <si>
-    <t>01/12/2025 19:34:35</t>
+    <t>01/12/2025 22:38:13</t>
   </si>
   <si>
     <t>הטופס מולא עם אותיות בשדה טלפון השני</t>
@@ -203,13 +203,13 @@
     <t>ניסיון שליחה עם טלפון שני לא תקין</t>
   </si>
   <si>
-    <t>01/12/2025 19:34:38</t>
+    <t>01/12/2025 22:38:16</t>
   </si>
   <si>
     <t>אימות טלפון שני לא תקין</t>
   </si>
   <si>
-    <t>01/12/2025 19:34:43</t>
+    <t>01/12/2025 22:38:21</t>
   </si>
   <si>
     <t>✓ המערכת מנעה שליחת טופס עם טלפון שני המכיל אותיות: "מספר הטלפון חייב להיות באורך של לפחות 10 ספרות." - הבדיקה עברה!</t>

</xml_diff>